<commit_message>
Updates in the notebook structure
</commit_message>
<xml_diff>
--- a/excel_parser/excel_files/workorder/2019 SUMAPPM Schedule Summit A.xlsx
+++ b/excel_parser/excel_files/workorder/2019 SUMAPPM Schedule Summit A.xlsx
@@ -526,7 +526,7 @@
     <t>weekly</t>
   </si>
   <si>
-    <t>D</t>
+    <t>d</t>
   </si>
   <si>
     <t>[10]</t>
@@ -562,7 +562,7 @@
     <t>[10, 23, 36, 49]</t>
   </si>
   <si>
-    <t>W</t>
+    <t>w</t>
   </si>
   <si>
     <t>[2, 15, 28, 41]</t>

</xml_diff>